<commit_message>
Add API of pickling for DataIO
</commit_message>
<xml_diff>
--- a/Python/Programs/ProgramTemplate_DM/Data/RAWDATA/CFG_KPI.xlsx
+++ b/Python/Programs/ProgramTemplate_DM/Data/RAWDATA/CFG_KPI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\Programs\ProgramTemplate_DM\Data\RAWDATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30EA74A-C23C-4C73-AA5C-FB4158BC9568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F39179-7F73-49AE-B176-AD1A52A5D228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09020CF4-9F51-448A-8C84-8E8C9A006B79}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{09020CF4-9F51-448A-8C84-8E8C9A006B79}"/>
   </bookViews>
   <sheets>
     <sheet name="KPIConfig" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Administrator</author>
+    <author>admin</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{1C576A35-4E69-4E49-BA55-B23F6203C14D}">
@@ -53,6 +54,32 @@
           <t xml:space="preserve">
 Rare cases:
 [1] When a Daily KPI starts on a workday whose previous calendar day is NOT workday, its MTD companion MUST start later than it. See detailed explanation in program &lt;310_MTD_mean.py&gt;</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="1" shapeId="0" xr:uid="{770F6008-8DC7-4601-92A1-C296D7385E7A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+PICKLE type is similar to SAS and can only store one DataFrame in one file</t>
         </r>
       </text>
     </comment>
@@ -89,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
   <si>
     <t>D_BGN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -212,22 +239,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>kpi2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>kpi1_fm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>kpi1_r15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>kpi2_r15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>kpi2_fm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -260,22 +275,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>mtd_kpi1_&amp;L_curdate..hdf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mtd_kpi2_&amp;L_curdate..hdf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r15_kpi1_&amp;L_curdate..hdf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r15_kpi2_&amp;L_curdate..hdf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>fm_agg_&amp;L_curMon..hdf</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -285,6 +284,26 @@
   </si>
   <si>
     <t>kpi2 mtd mean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PICKLE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mtd_kpi1_&amp;L_curdate..pkl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mtd_kpi2_&amp;L_curdate..pkl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r15_kpi1_&amp;L_curdate..pkl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r15_kpi2_&amp;L_curdate..pkl</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -387,9 +406,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主题">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -427,7 +446,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -533,7 +552,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -675,7 +694,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -686,7 +705,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -810,25 +829,19 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="G4" t="s">
         <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -842,25 +855,19 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="G5" t="s">
         <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>46</v>
-      </c>
-      <c r="I5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -880,16 +887,13 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
         <v>26</v>
       </c>
       <c r="H6" t="s">
-        <v>47</v>
-      </c>
-      <c r="I6" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -909,16 +913,13 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="G7" t="s">
         <v>26</v>
       </c>
       <c r="H7" t="s">
-        <v>48</v>
-      </c>
-      <c r="I7" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -944,10 +945,10 @@
         <v>26</v>
       </c>
       <c r="H8" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="I8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -973,10 +974,10 @@
         <v>26</v>
       </c>
       <c r="H9" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="I9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1020,7 +1021,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1031,7 +1032,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1042,7 +1043,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1053,7 +1054,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1064,7 +1065,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1075,7 +1076,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1086,7 +1087,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>